<commit_message>
update tests with bind and action helper
</commit_message>
<xml_diff>
--- a/sparkles-test.xlsx
+++ b/sparkles-test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gossi/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gossi/code/packages/sparkles-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E4F06E-D3EF-1D48-BEE2-1F7E16A1DAEE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7D25AF-8976-D64A-8704-4997ADC80E35}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="7620" windowWidth="28240" windowHeight="17560" xr2:uid="{E8DC77B4-C279-FF4A-A34B-EFB8B11024AE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>Invocation</t>
   </si>
@@ -48,9 +48,6 @@
     <t>&lt;Button /&gt;</t>
   </si>
   <si>
-    <t>&lt;Wurst/&gt;</t>
-  </si>
-  <si>
     <t>{{sub/wurst-thing}}</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Object Context</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>Assigned Object Context</t>
   </si>
   <si>
@@ -108,9 +102,6 @@
     <t>AssignChildComponent</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
     <t>src/ui/components/kaese/template.hbs</t>
   </si>
   <si>
@@ -126,28 +117,89 @@
     <t>Expected Not Found: components/sub/wurst/component.ts</t>
   </si>
   <si>
-    <t>Not Found:
+    <t>{{action}} helper</t>
+  </si>
+  <si>
+    <t>{{bind}} helper</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">components/kaese/template.hbs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2"/>
+        <rFont val="Calibri (Textkörper)_x0000_"/>
+      </rPr>
+      <t>* Given: components/kaese/template.hbs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">templates/components/kaese.hbs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2"/>
+        <rFont val="Calibri (Textkörper)_x0000_"/>
+      </rPr>
+      <t>* Given: templates/components/kaese/template.hbs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">components/kaese/template.hbs
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2"/>
+        <rFont val="Calibri (Textkörper)_x0000_"/>
+      </rPr>
+      <t>* Given: components/kaese/template.hbs
+* Given: templates/components/kaese/template.hbs</t>
+    </r>
+  </si>
+  <si>
+    <t>Classic: null
+MU: ObjectContextComponent</t>
+  </si>
+  <si>
+    <t>Object Context with Target</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>BindParentComponent</t>
+  </si>
+  <si>
+    <t>undefined</t>
+  </si>
+  <si>
+    <t>BindAssignParentComponent</t>
+  </si>
+  <si>
+    <t>Error: Specifier must not include a rootName, collection, or namespace</t>
+  </si>
+  <si>
+    <t>Error: Cannot find component wurst
 src/ui/components/sub/wurst/component.ts</t>
   </si>
   <si>
-    <t>components/kaese/template.hbs
-* Given: components/kaese/template.hbs</t>
-  </si>
-  <si>
-    <t>templates/components/kaese.hbs
-* Given: templates/components/kaese/template.hbs</t>
-  </si>
-  <si>
-    <t>components/kaese/template.hbs
-* Given: components/kaese/template.hbs
-* Given: templates/components/kaese/template.hbs</t>
+    <t>sub: &lt;Wurst/&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +227,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2"/>
+      <name val="Calibri (Textkörper)_x0000_"/>
     </font>
   </fonts>
   <fills count="5">
@@ -215,9 +272,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -227,17 +283,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -246,6 +297,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,226 +618,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24FD75E3-AD00-1344-8F49-D876E82FFF80}">
-  <dimension ref="A2:C24"/>
+  <dimension ref="A2:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" s="3" customFormat="1">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" ht="17">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34">
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="51">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="3" customFormat="1" ht="17">
+      <c r="A16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="34">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="C22" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17">
+      <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C24" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>26</v>
+      <c r="C25" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushed a test case for private vs public module collections in MU
</commit_message>
<xml_diff>
--- a/sparkles-test.xlsx
+++ b/sparkles-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gossi/code/packages/sparkles-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7D25AF-8976-D64A-8704-4997ADC80E35}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13809180-20AD-394C-8699-C4819CA5CF21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="7620" windowWidth="28240" windowHeight="17560" xr2:uid="{E8DC77B4-C279-FF4A-A34B-EFB8B11024AE}"/>
   </bookViews>
@@ -621,7 +621,7 @@
   <dimension ref="A2:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>